<commit_message>
All links open proper dialogs. Work needed on dialog js and jade files and some callbacks in client, etc. SS
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TG\TGv1000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="51">
   <si>
     <t>Function</t>
   </si>
@@ -248,12 +248,6 @@
   </si>
   <si>
     <t>jade created</t>
-  </si>
-  <si>
-    <t>js copied into</t>
-  </si>
-  <si>
-    <t>jade copied into</t>
   </si>
   <si>
     <t>js modified</t>
@@ -728,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,13 +739,11 @@
     <col min="7" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
@@ -768,33 +760,31 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>5</v>
@@ -809,556 +799,528 @@
         <v>8</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="J13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:13" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:13" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1369,28 +1331,26 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I1:L1"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
And generic rename is about done. SS
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="51">
   <si>
     <t>Function</t>
   </si>
@@ -307,12 +307,6 @@
     <t>Completion method created</t>
   </si>
   <si>
-    <t>Completion method written</t>
-  </si>
-  <si>
-    <t>tested</t>
-  </si>
-  <si>
     <t>Delete Confirmation (handles Type, Method, property, Event)</t>
   </si>
   <si>
@@ -380,6 +374,12 @@
   </si>
   <si>
     <t>Event.js</t>
+  </si>
+  <si>
+    <t>finished and tested</t>
+  </si>
+  <si>
+    <t>Completion or callback written</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,7 +728,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,29 +747,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -784,7 +787,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>5</v>
@@ -799,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -807,7 +810,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -816,23 +819,27 @@
         <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
@@ -840,7 +847,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
@@ -881,7 +888,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -920,7 +927,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>21</v>
@@ -929,23 +936,27 @@
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -953,7 +964,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>21</v>
@@ -962,23 +973,27 @@
         <v>21</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -986,7 +1001,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>21</v>
@@ -1019,7 +1034,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>21</v>
@@ -1052,7 +1067,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
@@ -1085,7 +1100,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -1094,21 +1109,25 @@
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -1116,7 +1135,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
@@ -1125,23 +1144,27 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -1149,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
@@ -1179,10 +1202,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
@@ -1191,23 +1214,27 @@
         <v>21</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -1215,7 +1242,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -1224,37 +1251,41 @@
         <v>21</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>21</v>
@@ -1263,7 +1294,7 @@
         <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
@@ -1272,22 +1303,26 @@
       <c r="J16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>21</v>
@@ -1296,7 +1331,7 @@
         <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
@@ -1305,16 +1340,20 @@
       <c r="J17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="M17" s="3"/>
     </row>
     <row r="20" spans="1:13" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>21</v>
@@ -1334,17 +1373,17 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filling in dialog code. SS
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="57">
   <si>
     <t>Function</t>
   </si>
@@ -380,6 +380,24 @@
   </si>
   <si>
     <t>Completion or callback written</t>
+  </si>
+  <si>
+    <t>Client has</t>
+  </si>
+  <si>
+    <t>self.addMethodToType(clMethod)</t>
+  </si>
+  <si>
+    <t>self.addMethodToTyoeFromDB(iMethodId)</t>
+  </si>
+  <si>
+    <t>self.addPropertyToType(clProperty)</t>
+  </si>
+  <si>
+    <t>self.addEventToType(clEvent)</t>
+  </si>
+  <si>
+    <t>These are called from NewMethod, SearchForMethod, NewProperty and NewEvent dialogs.</t>
   </si>
 </sst>
 </file>
@@ -428,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,6 +462,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,7 +749,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1018,7 +1039,9 @@
       <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +1074,9 @@
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1084,7 +1109,9 @@
       <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I10" s="1" t="s">
         <v>21</v>
       </c>
@@ -1189,7 +1216,9 @@
       <c r="G13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="I13" s="1" t="s">
         <v>21</v>
       </c>
@@ -1364,26 +1393,47 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I21" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="I22" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>46</v>
       </c>
+      <c r="I23" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>47</v>
       </c>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>48</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still need to write ScrollRegionV#m_functionAssureImageIsVisible.
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
   <si>
     <t>Function</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>see m_functionDeleteDialogHelper in code.js</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,27 +796,28 @@
     <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="69.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -853,8 +857,11 @@
       <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -891,7 +898,7 @@
       </c>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -932,7 +939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -971,7 +978,7 @@
       </c>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1008,7 +1015,7 @@
       </c>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1052,7 @@
       </c>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1087,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1115,7 +1122,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1150,7 +1157,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1185,7 +1192,7 @@
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1229,7 @@
       </c>
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1257,7 +1264,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1294,7 +1301,7 @@
       </c>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1331,7 +1338,7 @@
       </c>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1440,7 @@
       <c r="M20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N20" s="7" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete type is done and I'm done for the day.
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11790" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,9 +431,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Validate that it's deletable before opening dialog.</t>
-  </si>
-  <si>
     <t>see m_functionDeleteDialogHelper in Type.js</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>"new_" + type.name</t>
+  </si>
+  <si>
+    <t>Validate that it's deletable before opening dialog. Will work once Ken adds code to app Type::initialize.</t>
   </si>
 </sst>
 </file>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -922,7 +922,7 @@
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.1796875" customWidth="1"/>
-    <col min="15" max="15" width="64.81640625" style="6" customWidth="1"/>
+    <col min="15" max="15" width="64.81640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -990,7 +990,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1029,8 +1029,8 @@
       <c r="N3" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="6" t="s">
-        <v>67</v>
+      <c r="O3" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -1156,7 +1156,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1195,8 +1195,8 @@
       <c r="N7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="O7" s="6" t="s">
-        <v>67</v>
+      <c r="O7" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1348,7 +1348,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1387,8 +1387,8 @@
       <c r="N12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="O12" s="6" t="s">
-        <v>67</v>
+      <c r="O12" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -1469,7 +1469,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1508,8 +1508,8 @@
       <c r="N15" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>67</v>
+      <c r="O15" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
@@ -1677,7 +1677,7 @@
         <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
@@ -1710,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -1723,147 +1723,147 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>-1</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
         <v>74</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>76</v>
-      </c>
-      <c r="F16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1871,60 +1871,60 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
         <v>93</v>
-      </c>
-      <c r="C26" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost done with Rename (Type, Method, Event). SS
</commit_message>
<xml_diff>
--- a/Dialogs.xlsx
+++ b/Dialogs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11790"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11790" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -227,8 +227,114 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Gerald Rubin</author>
+  </authors>
+  <commentList>
+    <comment ref="S10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gerald Rubin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In Types.js#addItem</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gerald Rubin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In Client.js#addMethodToActiveType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gerald Rubin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+But Code.js#m_functionAdd_Type_Property needs examination by Ken</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gerald Rubin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In Client.js#addEventToActiveType, but routine is commented out in Code.js#m_functionAdd_Type_Event</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="119">
   <si>
     <t>Function</t>
   </si>
@@ -543,6 +649,48 @@
   </si>
   <si>
     <t>Validate that it's deletable before opening dialog. Will work once Ken adds code to app Type::initialize.</t>
+  </si>
+  <si>
+    <t>Add Type</t>
+  </si>
+  <si>
+    <t>Rename Type</t>
+  </si>
+  <si>
+    <t>Rename Method</t>
+  </si>
+  <si>
+    <t>Call Client check for duplicate in Save func</t>
+  </si>
+  <si>
+    <t>Client routine written</t>
+  </si>
+  <si>
+    <t>Types routine written</t>
+  </si>
+  <si>
+    <t>Comics routine written</t>
+  </si>
+  <si>
+    <t>Is it correct?</t>
+  </si>
+  <si>
+    <t>Replace in array</t>
+  </si>
+  <si>
+    <t>Replace in code</t>
+  </si>
+  <si>
+    <t>Add to array</t>
+  </si>
+  <si>
+    <t>Add to code</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>incomplete</t>
   </si>
 </sst>
 </file>
@@ -591,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,6 +768,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -904,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -926,22 +1086,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:15" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1707,11 +1867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1719,14 +1879,21 @@
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.453125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.54296875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.36328125" style="11" customWidth="1"/>
+    <col min="16" max="18" width="8.7265625" style="11"/>
+    <col min="19" max="19" width="10.453125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>73</v>
       </c>
@@ -1740,7 +1907,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>69</v>
       </c>
@@ -1757,7 +1924,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>70</v>
       </c>
@@ -1774,7 +1941,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>71</v>
       </c>
@@ -1791,7 +1958,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>72</v>
       </c>
@@ -1808,17 +1975,195 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="L9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>73</v>
       </c>
@@ -1831,8 +2176,35 @@
       <c r="F16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>69</v>
       </c>
@@ -1848,8 +2220,29 @@
       <c r="F17" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="R17" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>72</v>
       </c>
@@ -1866,15 +2259,29 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F19" s="10"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="N19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="O19" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>91</v>
       </c>
@@ -1882,7 +2289,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>92</v>
       </c>
@@ -1890,12 +2297,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>91</v>
       </c>
@@ -1903,7 +2310,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>97</v>
       </c>
@@ -1911,7 +2318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>98</v>
       </c>
@@ -1919,7 +2326,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>99</v>
       </c>
@@ -1929,5 +2336,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>